<commit_message>
added downloads data preperation script
</commit_message>
<xml_diff>
--- a/generator/data/generated_business_variable_map.xlsx
+++ b/generator/data/generated_business_variable_map.xlsx
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -658,7 +658,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6">
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E7" t="n">
         <v>3</v>
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8">
@@ -766,7 +766,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E8" t="n">
         <v>4</v>
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9">
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E9" t="n">
         <v>5</v>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E10" t="n">
         <v>6</v>
@@ -878,7 +878,7 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11">
@@ -898,7 +898,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E11" t="n">
         <v>7</v>
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E12" t="n">
         <v>8</v>
@@ -966,7 +966,7 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13">
@@ -986,7 +986,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E13" t="n">
         <v>9</v>
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E14" t="n">
         <v>10</v>
@@ -1054,7 +1054,7 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15">
@@ -1074,7 +1074,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E15" t="n">
         <v>11</v>
@@ -1098,7 +1098,7 @@
         </is>
       </c>
       <c r="J15" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16">
@@ -1118,7 +1118,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E16" t="n">
         <v>12</v>
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="J16" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E17" t="n">
         <v>13</v>
@@ -1186,7 +1186,7 @@
         </is>
       </c>
       <c r="J17" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18">
@@ -1206,7 +1206,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E18" t="n">
         <v>14</v>
@@ -1230,7 +1230,7 @@
         </is>
       </c>
       <c r="J18" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19">
@@ -1250,7 +1250,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E19" t="n">
         <v>15</v>
@@ -1274,7 +1274,7 @@
         </is>
       </c>
       <c r="J19" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20">
@@ -1294,7 +1294,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E20" t="n">
         <v>16</v>
@@ -1318,7 +1318,7 @@
         </is>
       </c>
       <c r="J20" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21">
@@ -1338,7 +1338,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E21" t="n">
         <v>17</v>
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="J21" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E22" t="n">
         <v>18</v>
@@ -1406,7 +1406,7 @@
         </is>
       </c>
       <c r="J22" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23">
@@ -1426,7 +1426,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E23" t="n">
         <v>19</v>
@@ -1450,7 +1450,7 @@
         </is>
       </c>
       <c r="J23" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24">
@@ -1494,7 +1494,7 @@
         </is>
       </c>
       <c r="J24" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25">
@@ -1538,7 +1538,7 @@
         </is>
       </c>
       <c r="J25" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26">
@@ -1558,7 +1558,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E26" t="n">
         <v>22</v>
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="J26" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27">
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E27" t="n">
         <v>23</v>
@@ -1626,7 +1626,7 @@
         </is>
       </c>
       <c r="J27" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28">
@@ -1646,7 +1646,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E28" t="n">
         <v>24</v>
@@ -1670,7 +1670,7 @@
         </is>
       </c>
       <c r="J28" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E29" t="n">
         <v>25</v>
@@ -1714,7 +1714,7 @@
         </is>
       </c>
       <c r="J29" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30">
@@ -1734,7 +1734,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E30" t="n">
         <v>26</v>
@@ -1758,7 +1758,7 @@
         </is>
       </c>
       <c r="J30" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31">
@@ -1778,7 +1778,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E31" t="n">
         <v>27</v>
@@ -1802,7 +1802,7 @@
         </is>
       </c>
       <c r="J31" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32">
@@ -1846,7 +1846,7 @@
         </is>
       </c>
       <c r="J32" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33">
@@ -1866,7 +1866,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E33" t="n">
         <v>29</v>
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="J33" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34">
@@ -1910,7 +1910,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E34" t="n">
         <v>30</v>
@@ -1934,7 +1934,7 @@
         </is>
       </c>
       <c r="J34" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35">
@@ -1954,7 +1954,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E35" t="n">
         <v>31</v>
@@ -1978,7 +1978,7 @@
         </is>
       </c>
       <c r="J35" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36">
@@ -1998,7 +1998,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E36" t="n">
         <v>32</v>
@@ -2022,7 +2022,7 @@
         </is>
       </c>
       <c r="J36" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37">
@@ -2042,7 +2042,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E37" t="n">
         <v>33</v>
@@ -2066,7 +2066,7 @@
         </is>
       </c>
       <c r="J37" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38">
@@ -2110,7 +2110,7 @@
         </is>
       </c>
       <c r="J38" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39">
@@ -2154,7 +2154,7 @@
         </is>
       </c>
       <c r="J39" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40">
@@ -2198,7 +2198,7 @@
         </is>
       </c>
       <c r="J40" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>